<commit_message>
Agregados IDs y creadas relaciones en la tabla
</commit_message>
<xml_diff>
--- a/data/bga-metadatos.xlsx
+++ b/data/bga-metadatos.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="43760" yWindow="1800" windowWidth="46320" windowHeight="14880" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="48020" yWindow="1300" windowWidth="46320" windowHeight="14880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="obras" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
   <si>
     <t>Título</t>
   </si>
@@ -60,12 +60,6 @@
     <t>Periódico</t>
   </si>
   <si>
-    <t>Fecha referente</t>
-  </si>
-  <si>
-    <t>Titulo referente</t>
-  </si>
-  <si>
     <t>Doble suicidio en "El Sisga"</t>
   </si>
   <si>
@@ -90,15 +84,6 @@
     <t>Mayo 24 del 96</t>
   </si>
   <si>
-    <t>archivo referente</t>
-  </si>
-  <si>
-    <t>Una indígena y su hijo murieron en persecución;Láminas de paisajes latinoamericanos</t>
-  </si>
-  <si>
-    <t>el-paraiso.jpg, laminas-paisajes.jpg</t>
-  </si>
-  <si>
     <t>Zócalo de la tragedia</t>
   </si>
   <si>
@@ -111,9 +96,6 @@
     <t>zocalo-tragedia.jpg</t>
   </si>
   <si>
-    <t>Exmilitar Mata a la Ezposa de su Amigo y se Suicida</t>
-  </si>
-  <si>
     <t>exmilitar-mata-esposa.jpg</t>
   </si>
   <si>
@@ -124,6 +106,18 @@
   </si>
   <si>
     <t>laminas-paisajes.jpg</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Referentes</t>
+  </si>
+  <si>
+    <t>2,3</t>
+  </si>
+  <si>
+    <t>Exmilitar Mata a la Esposa de su Amigo y se Suicida</t>
   </si>
 </sst>
 </file>
@@ -447,132 +441,111 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:I3"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="41.1640625" customWidth="1"/>
-    <col min="2" max="2" width="22.1640625" customWidth="1"/>
-    <col min="3" max="3" width="18.5" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" customWidth="1"/>
-    <col min="5" max="5" width="21.33203125" customWidth="1"/>
-    <col min="6" max="6" width="27.33203125" customWidth="1"/>
-    <col min="7" max="8" width="19.33203125" customWidth="1"/>
-    <col min="9" max="9" width="22.1640625" customWidth="1"/>
+    <col min="2" max="2" width="41.1640625" customWidth="1"/>
+    <col min="3" max="3" width="22.1640625" customWidth="1"/>
+    <col min="4" max="4" width="18.5" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" customWidth="1"/>
+    <col min="6" max="6" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>1965</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3">
+        <v>1997</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4">
+        <v>1983</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2">
-        <v>1965</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3">
-        <v>1997</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="F4" t="s">
         <v>21</v>
       </c>
-      <c r="G3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4">
-        <v>1983</v>
-      </c>
-      <c r="C4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4" t="s">
-        <v>28</v>
+      <c r="G4">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -582,68 +555,91 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="53.33203125" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" customWidth="1"/>
-    <col min="3" max="3" width="40.1640625" customWidth="1"/>
-    <col min="4" max="4" width="56.83203125" customWidth="1"/>
+    <col min="2" max="2" width="53.33203125" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" customWidth="1"/>
+    <col min="4" max="4" width="40.1640625" customWidth="1"/>
+    <col min="5" max="5" width="56.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" t="s">
-        <v>31</v>
+      <c r="E5" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modificación en nombres de columnas, agregada columna de relación con  obras en referentes
</commit_message>
<xml_diff>
--- a/data/bga-metadatos.xlsx
+++ b/data/bga-metadatos.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10910"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmart/HD/taller-control-versiones/bga-cat/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gemartin/herramientas-digitales/modulo-db/bga-cat/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{175234C0-5EB0-4645-8054-E8285D61A4FA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43960" yWindow="10880" windowWidth="34080" windowHeight="12840" tabRatio="500"/>
+    <workbookView xWindow="2840" yWindow="2340" windowWidth="23920" windowHeight="12460" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="obras" sheetId="1" r:id="rId1"/>
+    <sheet name="obra" sheetId="1" r:id="rId1"/>
     <sheet name="refentes" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,10 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
-  <si>
-    <t>Archivo</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
   <si>
     <t>Los Suicidas del Sisga No 1</t>
   </si>
@@ -81,43 +79,52 @@
     <t>ID</t>
   </si>
   <si>
-    <t>Referentes</t>
-  </si>
-  <si>
     <t>2,3</t>
   </si>
   <si>
     <t>Exmilitar Mata a la Esposa de su Amigo y se Suicida</t>
   </si>
   <si>
-    <t>ancho cm</t>
-  </si>
-  <si>
-    <t>alto cm</t>
-  </si>
-  <si>
-    <t>Publisher</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>Creator</t>
-  </si>
-  <si>
     <t>Beatriz González</t>
   </si>
   <si>
-    <t>Format.medium</t>
+    <t>date</t>
+  </si>
+  <si>
+    <t>ancho</t>
+  </si>
+  <si>
+    <t>alto</t>
+  </si>
+  <si>
+    <t>medium</t>
+  </si>
+  <si>
+    <t>archivo</t>
+  </si>
+  <si>
+    <t>referentes</t>
+  </si>
+  <si>
+    <t>creator</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>publisher</t>
+  </si>
+  <si>
+    <t>obra</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -155,10 +162,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -168,6 +176,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -435,11 +446,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -447,7 +458,8 @@
     <col min="1" max="1" width="6.5" customWidth="1"/>
     <col min="2" max="2" width="19.33203125" customWidth="1"/>
     <col min="3" max="3" width="41.1640625" customWidth="1"/>
-    <col min="4" max="5" width="22.1640625" customWidth="1"/>
+    <col min="4" max="4" width="22.1640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="22.1640625" customWidth="1"/>
     <col min="6" max="6" width="18.5" customWidth="1"/>
     <col min="7" max="7" width="18.33203125" customWidth="1"/>
     <col min="8" max="8" width="21.33203125" customWidth="1"/>
@@ -455,16 +467,16 @@
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>20</v>
@@ -473,13 +485,13 @@
         <v>21</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -487,13 +499,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1965</v>
+        <v>0</v>
+      </c>
+      <c r="D2" s="3">
+        <v>23743</v>
       </c>
       <c r="E2">
         <v>120</v>
@@ -502,10 +514,10 @@
         <v>100</v>
       </c>
       <c r="G2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
         <v>2</v>
-      </c>
-      <c r="H2" t="s">
-        <v>3</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -516,13 +528,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3">
-        <v>1997</v>
+        <v>5</v>
+      </c>
+      <c r="D3" s="3">
+        <v>35431</v>
       </c>
       <c r="E3">
         <v>160</v>
@@ -531,13 +543,13 @@
         <v>45</v>
       </c>
       <c r="G3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -545,13 +557,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4">
-        <v>1983</v>
+        <v>8</v>
+      </c>
+      <c r="D4" s="3">
+        <v>30317</v>
       </c>
       <c r="E4">
         <v>100</v>
@@ -560,10 +572,10 @@
         <v>70</v>
       </c>
       <c r="G4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" t="s">
         <v>10</v>
-      </c>
-      <c r="H4" t="s">
-        <v>11</v>
       </c>
       <c r="I4">
         <v>4</v>
@@ -575,92 +587,107 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="53.33203125" customWidth="1"/>
-    <col min="3" max="3" width="24.6640625" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" style="3" customWidth="1"/>
     <col min="4" max="4" width="40.1640625" customWidth="1"/>
     <col min="5" max="5" width="56.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3">
+        <v>23922</v>
+      </c>
+      <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2">
-        <v>23922</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
       <c r="E2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="2">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3">
         <v>35209</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
         <v>14</v>
       </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>